<commit_message>
Changed 1_UPI to 4_UPI and 6_PAR to 4_PAR.
</commit_message>
<xml_diff>
--- a/doc/LCI_IEDC_Correspondences_V1.xlsx
+++ b/doc/LCI_IEDC_Correspondences_V1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kuczenski et al. model to IEDC" sheetId="1" r:id="rId1"/>
@@ -937,18 +937,12 @@
     <t>insert for current property and exchange/flow</t>
   </si>
   <si>
-    <t>6_TC_&lt;database name&gt;_&lt;activity id&gt;</t>
-  </si>
-  <si>
     <t>Transfer coefficients</t>
   </si>
   <si>
     <t>separate dataset, cf. 'TransferCoefficient' datatype below</t>
   </si>
   <si>
-    <t>6_TC_</t>
-  </si>
-  <si>
     <t>data.aspect1 (exchange id)</t>
   </si>
   <si>
@@ -1204,9 +1198,6 @@
     <t>data.aspect9</t>
   </si>
   <si>
-    <t>Not convertible (can be added as comment, or referenced via DOI)</t>
-  </si>
-  <si>
     <t>geographical scope of activity dataset</t>
   </si>
   <si>
@@ -1441,12 +1432,6 @@
     <t>material_group</t>
   </si>
   <si>
-    <t>6_PAR_&lt;database name&gt;_&lt;activity id&gt;</t>
-  </si>
-  <si>
-    <t>6_PAR_</t>
-  </si>
-  <si>
     <t>6_FPR_UnitPrices_&lt;database name&gt;</t>
   </si>
   <si>
@@ -1583,6 +1568,21 @@
   </si>
   <si>
     <t>Reference:</t>
+  </si>
+  <si>
+    <t>4_TC_&lt;database name&gt;_&lt;activity id&gt;</t>
+  </si>
+  <si>
+    <t>4_PAR_&lt;database name&gt;_&lt;activity id&gt;</t>
+  </si>
+  <si>
+    <t>Not convertible (can be added as comment, or referenced via DOI). Can be stored as dictionary in comment field instead.</t>
+  </si>
+  <si>
+    <t>4_TC_</t>
+  </si>
+  <si>
+    <t>4_PAR_</t>
   </si>
 </sst>
 </file>
@@ -2162,7 +2162,7 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -2451,12 +2451,12 @@
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="5" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -2469,8 +2469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q339"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I202" sqref="I202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2485,7 +2485,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B1" s="4"/>
       <c r="E1" s="5"/>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
@@ -2740,7 +2740,7 @@
         <v>121</v>
       </c>
       <c r="J17" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2751,7 +2751,7 @@
         <v>113</v>
       </c>
       <c r="J18" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2762,7 +2762,7 @@
         <v>122</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>394</v>
+        <v>518</v>
       </c>
       <c r="L19" t="s">
         <v>109</v>
@@ -2837,18 +2837,18 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J26" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="J27" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -2867,7 +2867,7 @@
         <v>144</v>
       </c>
       <c r="D30" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L30" t="s">
         <v>7</v>
@@ -2878,7 +2878,7 @@
         <v>145</v>
       </c>
       <c r="D31" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -2886,20 +2886,20 @@
         <v>146</v>
       </c>
       <c r="D32" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="34" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="35"/>
       <c r="C34" s="5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="35"/>
       <c r="C35" s="20" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D35" s="17">
         <v>1</v>
@@ -2951,10 +2951,10 @@
         <v>69</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H36" s="34" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>71</v>
@@ -2981,10 +2981,10 @@
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="35"/>
       <c r="C37" s="22" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>132</v>
@@ -2993,13 +2993,13 @@
         <v>73</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>73</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>133</v>
@@ -3033,7 +3033,7 @@
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="35"/>
       <c r="C39" s="21" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>66</v>
@@ -3045,10 +3045,10 @@
         <v>69</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H39" s="34" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I39" s="11" t="s">
         <v>71</v>
@@ -3075,10 +3075,10 @@
     <row r="40" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B40" s="35"/>
       <c r="C40" s="22" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>132</v>
@@ -3087,16 +3087,16 @@
         <v>73</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>73</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
@@ -3127,7 +3127,7 @@
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="35"/>
       <c r="C42" s="21" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>66</v>
@@ -3142,16 +3142,16 @@
         <v>69</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I42" s="34" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="J42" s="11" t="s">
         <v>71</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="L42" s="11" t="s">
         <v>72</v>
@@ -3176,25 +3176,25 @@
         <v>130</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F43" s="36" t="s">
+        <v>457</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>458</v>
+      </c>
+      <c r="H43" s="36" t="s">
         <v>460</v>
       </c>
-      <c r="G43" s="36" t="s">
-        <v>461</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>463</v>
-      </c>
       <c r="I43" s="36" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="K43" s="12" t="s">
         <v>75</v>
@@ -3241,10 +3241,10 @@
         <v>69</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H45" s="34" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I45" s="11" t="s">
         <v>71</v>
@@ -3274,7 +3274,7 @@
         <v>131</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>132</v>
@@ -3283,16 +3283,16 @@
         <v>73</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H46" s="12" t="s">
         <v>73</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
@@ -3323,10 +3323,10 @@
     <row r="48" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B48" s="35"/>
       <c r="C48" s="21" t="s">
-        <v>473</v>
+        <v>517</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>70</v>
@@ -3362,16 +3362,16 @@
         <v>103</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
@@ -3405,10 +3405,10 @@
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B51" s="35"/>
       <c r="C51" s="21" t="s">
-        <v>305</v>
+        <v>516</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>70</v>
@@ -3417,16 +3417,16 @@
         <v>71</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="K51" s="11"/>
       <c r="L51" s="11"/>
@@ -3447,28 +3447,28 @@
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B52" s="35"/>
       <c r="C52" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G52" s="37" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H52" s="36" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J52" s="12" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
@@ -3499,7 +3499,7 @@
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B54" s="35"/>
       <c r="C54" s="21" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D54" s="11" t="s">
         <v>66</v>
@@ -3520,7 +3520,7 @@
         <v>72</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="K54" s="11"/>
       <c r="L54" s="11"/>
@@ -3544,25 +3544,25 @@
         <v>208</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="F55" s="15" t="s">
         <v>202</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I55" s="15" t="s">
         <v>133</v>
       </c>
       <c r="J55" s="15" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="K55" s="15"/>
       <c r="L55" s="15"/>
@@ -3574,7 +3574,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="28" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B57" s="28"/>
       <c r="C57" s="28"/>
@@ -3589,13 +3589,13 @@
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30"/>
       <c r="B59" s="30" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="L59" s="5" t="s">
         <v>6</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B60" s="30" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="J60" s="6" t="s">
         <v>13</v>
@@ -3614,7 +3614,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B61" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="J61" s="6" t="s">
         <v>14</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B64" s="32" t="s">
         <v>1</v>
@@ -4200,7 +4200,7 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="33" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B110" s="28" t="s">
         <v>135</v>
@@ -4539,10 +4539,10 @@
         <v>4</v>
       </c>
       <c r="I132" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J132" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="133" spans="3:12" x14ac:dyDescent="0.3">
@@ -4570,7 +4570,7 @@
         <v>4</v>
       </c>
       <c r="I134" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J134" s="6" t="s">
         <v>303</v>
@@ -4626,10 +4626,10 @@
         <v>284</v>
       </c>
       <c r="J139" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L139" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="140" spans="3:12" x14ac:dyDescent="0.3">
@@ -4643,10 +4643,10 @@
         <v>284</v>
       </c>
       <c r="J140" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L140" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="141" spans="3:12" x14ac:dyDescent="0.3">
@@ -4688,10 +4688,10 @@
         <v>284</v>
       </c>
       <c r="J143" s="6" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="L143" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="144" spans="3:12" x14ac:dyDescent="0.3">
@@ -4902,7 +4902,7 @@
     </row>
     <row r="158" spans="4:12" x14ac:dyDescent="0.3">
       <c r="H158" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I158" t="s">
         <v>284</v>
@@ -4911,7 +4911,7 @@
         <v>220</v>
       </c>
       <c r="L158" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="159" spans="4:12" x14ac:dyDescent="0.3">
@@ -4923,7 +4923,7 @@
         <v>184</v>
       </c>
       <c r="L159" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="160" spans="4:12" x14ac:dyDescent="0.3">
@@ -4931,10 +4931,10 @@
         <v>284</v>
       </c>
       <c r="J160" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="L160" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="161" spans="3:12" x14ac:dyDescent="0.3">
@@ -4942,10 +4942,10 @@
         <v>284</v>
       </c>
       <c r="J161" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L161" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="162" spans="3:12" x14ac:dyDescent="0.3">
@@ -4953,10 +4953,10 @@
         <v>284</v>
       </c>
       <c r="J162" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L162" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="163" spans="3:12" x14ac:dyDescent="0.3">
@@ -4967,7 +4967,7 @@
         <v>160</v>
       </c>
       <c r="L163" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="164" spans="3:12" x14ac:dyDescent="0.3">
@@ -4978,7 +4978,7 @@
         <v>220</v>
       </c>
       <c r="L164" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="165" spans="3:12" x14ac:dyDescent="0.3">
@@ -4989,7 +4989,7 @@
         <v>185</v>
       </c>
       <c r="L165" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="166" spans="3:12" x14ac:dyDescent="0.3">
@@ -5000,7 +5000,7 @@
         <v>207</v>
       </c>
       <c r="L166" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="167" spans="3:12" x14ac:dyDescent="0.3">
@@ -5011,7 +5011,7 @@
         <v>178</v>
       </c>
       <c r="L167" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="168" spans="3:12" x14ac:dyDescent="0.3">
@@ -5022,7 +5022,7 @@
         <v>179</v>
       </c>
       <c r="L168" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="169" spans="3:12" x14ac:dyDescent="0.3">
@@ -5030,10 +5030,10 @@
         <v>285</v>
       </c>
       <c r="J169" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L169" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="171" spans="3:12" x14ac:dyDescent="0.3">
@@ -5052,10 +5052,10 @@
         <v>284</v>
       </c>
       <c r="J172" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L172" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="173" spans="3:12" x14ac:dyDescent="0.3">
@@ -5069,10 +5069,10 @@
         <v>284</v>
       </c>
       <c r="J173" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L173" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="174" spans="3:12" x14ac:dyDescent="0.3">
@@ -5117,7 +5117,7 @@
         <v>184</v>
       </c>
       <c r="L176" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="177" spans="3:12" x14ac:dyDescent="0.3">
@@ -5144,7 +5144,7 @@
     <row r="179" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D179" s="3"/>
       <c r="H179" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I179" t="s">
         <v>284</v>
@@ -5153,7 +5153,7 @@
         <v>220</v>
       </c>
       <c r="L179" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="180" spans="3:12" x14ac:dyDescent="0.3">
@@ -5166,7 +5166,7 @@
         <v>184</v>
       </c>
       <c r="L180" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="181" spans="3:12" x14ac:dyDescent="0.3">
@@ -5175,10 +5175,10 @@
         <v>284</v>
       </c>
       <c r="J181" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="L181" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="182" spans="3:12" x14ac:dyDescent="0.3">
@@ -5187,10 +5187,10 @@
         <v>284</v>
       </c>
       <c r="J182" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L182" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="183" spans="3:12" x14ac:dyDescent="0.3">
@@ -5199,10 +5199,10 @@
         <v>284</v>
       </c>
       <c r="J183" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L183" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="185" spans="3:12" x14ac:dyDescent="0.3">
@@ -5218,13 +5218,13 @@
         <v>4</v>
       </c>
       <c r="I186" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J186" s="6" t="s">
         <v>207</v>
       </c>
       <c r="L186" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="187" spans="3:12" x14ac:dyDescent="0.3">
@@ -5235,7 +5235,7 @@
         <v>4</v>
       </c>
       <c r="I187" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J187" s="6" t="s">
         <v>151</v>
@@ -5252,7 +5252,7 @@
         <v>20</v>
       </c>
       <c r="I188" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J188" s="6" t="s">
         <v>151</v>
@@ -5269,7 +5269,7 @@
         <v>4</v>
       </c>
       <c r="I189" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J189" s="6" t="s">
         <v>158</v>
@@ -5286,7 +5286,7 @@
         <v>20</v>
       </c>
       <c r="I190" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J190" t="s">
         <v>161</v>
@@ -5331,7 +5331,7 @@
         <v>20</v>
       </c>
       <c r="I193" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J193" s="6" t="s">
         <v>151</v>
@@ -5348,7 +5348,7 @@
         <v>20</v>
       </c>
       <c r="I194" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J194" s="6" t="s">
         <v>151</v>
@@ -5365,7 +5365,7 @@
         <v>20</v>
       </c>
       <c r="I195" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J195" s="6" t="s">
         <v>151</v>
@@ -5382,7 +5382,7 @@
         <v>20</v>
       </c>
       <c r="I196" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J196" s="6" t="s">
         <v>151</v>
@@ -5399,7 +5399,7 @@
         <v>20</v>
       </c>
       <c r="I197" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J197" s="6" t="s">
         <v>174</v>
@@ -5413,38 +5413,38 @@
     </row>
     <row r="199" spans="3:12" x14ac:dyDescent="0.3">
       <c r="H199" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I199" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J199" t="s">
         <v>160</v>
       </c>
       <c r="L199" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="200" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I200" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J200" t="s">
         <v>220</v>
       </c>
       <c r="L200" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="201" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I201" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="J201" t="s">
         <v>185</v>
       </c>
       <c r="L201" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="203" spans="3:12" x14ac:dyDescent="0.3">
@@ -5460,13 +5460,13 @@
         <v>4</v>
       </c>
       <c r="I204" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J204" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L204" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="205" spans="3:12" x14ac:dyDescent="0.3">
@@ -5477,7 +5477,7 @@
         <v>20</v>
       </c>
       <c r="I205" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J205" s="6" t="s">
         <v>151</v>
@@ -5494,7 +5494,7 @@
         <v>4</v>
       </c>
       <c r="I206" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J206" s="6" t="s">
         <v>151</v>
@@ -5511,7 +5511,7 @@
         <v>20</v>
       </c>
       <c r="I207" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J207" s="6" t="s">
         <v>151</v>
@@ -5528,7 +5528,7 @@
         <v>4</v>
       </c>
       <c r="I208" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J208" s="6" t="s">
         <v>151</v>
@@ -5545,7 +5545,7 @@
         <v>4</v>
       </c>
       <c r="I209" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J209" s="6" t="s">
         <v>151</v>
@@ -5562,7 +5562,7 @@
         <v>20</v>
       </c>
       <c r="I210" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J210" s="6" t="s">
         <v>151</v>
@@ -5593,7 +5593,7 @@
         <v>4</v>
       </c>
       <c r="I212" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J212" s="6" t="s">
         <v>158</v>
@@ -5610,7 +5610,7 @@
         <v>4</v>
       </c>
       <c r="I213" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J213" s="6" t="s">
         <v>162</v>
@@ -5627,7 +5627,7 @@
         <v>4</v>
       </c>
       <c r="I214" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J214" t="s">
         <v>161</v>
@@ -5641,71 +5641,71 @@
     </row>
     <row r="216" spans="3:12" x14ac:dyDescent="0.3">
       <c r="H216" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I216" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J216" s="6" t="s">
         <v>160</v>
       </c>
       <c r="L216" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="217" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I217" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J217" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L217" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="218" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I218" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J218" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="L218" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="219" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I219" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J219" s="6" t="s">
         <v>207</v>
       </c>
       <c r="L219" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="220" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I220" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J220" s="6" t="s">
         <v>178</v>
       </c>
       <c r="L220" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="221" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I221" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J221" s="6" t="s">
         <v>179</v>
       </c>
       <c r="L221" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="222" spans="3:12" x14ac:dyDescent="0.3">
@@ -5846,10 +5846,10 @@
         <v>4</v>
       </c>
       <c r="I235" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J235" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="K235" t="s">
         <v>302</v>
@@ -5866,7 +5866,7 @@
         <v>20</v>
       </c>
       <c r="I236" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J236" t="s">
         <v>161</v>
@@ -5911,7 +5911,7 @@
         <v>4</v>
       </c>
       <c r="I239" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J239" s="6" t="s">
         <v>158</v>
@@ -5928,7 +5928,7 @@
         <v>20</v>
       </c>
       <c r="I240" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J240" s="6" t="s">
         <v>151</v>
@@ -5945,7 +5945,7 @@
         <v>20</v>
       </c>
       <c r="I241" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J241" s="6" t="s">
         <v>151</v>
@@ -5962,7 +5962,7 @@
         <v>20</v>
       </c>
       <c r="I242" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J242" s="6" t="s">
         <v>151</v>
@@ -5979,7 +5979,7 @@
         <v>20</v>
       </c>
       <c r="I243" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J243" s="6" t="s">
         <v>151</v>
@@ -5996,7 +5996,7 @@
         <v>20</v>
       </c>
       <c r="I244" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J244" s="6" t="s">
         <v>174</v>
@@ -6083,7 +6083,7 @@
         <v>20</v>
       </c>
       <c r="I250" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J250" s="6" t="s">
         <v>151</v>
@@ -6099,76 +6099,76 @@
     <row r="252" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D252" s="3"/>
       <c r="H252" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I252" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J252" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L252" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="253" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D253" s="3"/>
       <c r="I253" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J253" s="6" t="s">
         <v>220</v>
       </c>
       <c r="L253" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="254" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D254" s="3"/>
       <c r="I254" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J254" s="6" t="s">
         <v>185</v>
       </c>
       <c r="L254" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="255" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D255" s="3"/>
       <c r="I255" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J255" s="6" t="s">
         <v>207</v>
       </c>
       <c r="L255" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="256" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D256" s="3"/>
       <c r="I256" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J256" s="6" t="s">
         <v>178</v>
       </c>
       <c r="L256" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="257" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D257" s="3"/>
       <c r="I257" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J257" s="6" t="s">
         <v>179</v>
       </c>
       <c r="L257" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="259" spans="3:12" x14ac:dyDescent="0.3">
@@ -6178,19 +6178,19 @@
     </row>
     <row r="260" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D260" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E260" t="s">
         <v>4</v>
       </c>
       <c r="I260" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J260" s="6" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="L260" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="261" spans="3:12" x14ac:dyDescent="0.3">
@@ -6201,13 +6201,13 @@
         <v>4</v>
       </c>
       <c r="I261" t="s">
+        <v>519</v>
+      </c>
+      <c r="J261" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="L261" t="s">
         <v>308</v>
-      </c>
-      <c r="J261" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="L261" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="262" spans="3:12" x14ac:dyDescent="0.3">
@@ -6218,7 +6218,7 @@
         <v>4</v>
       </c>
       <c r="I262" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J262" s="6" t="s">
         <v>158</v>
@@ -6235,7 +6235,7 @@
         <v>20</v>
       </c>
       <c r="I263" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J263" s="6" t="s">
         <v>151</v>
@@ -6252,7 +6252,7 @@
         <v>20</v>
       </c>
       <c r="I264" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J264" s="6" t="s">
         <v>151</v>
@@ -6269,7 +6269,7 @@
         <v>20</v>
       </c>
       <c r="I265" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J265" s="6" t="s">
         <v>174</v>
@@ -6356,7 +6356,7 @@
         <v>20</v>
       </c>
       <c r="I271" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J271" s="6" t="s">
         <v>151</v>
@@ -6372,98 +6372,98 @@
     <row r="273" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D273" s="3"/>
       <c r="H273" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I273" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J273" s="6" t="s">
         <v>160</v>
       </c>
       <c r="L273" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D274" s="3"/>
       <c r="I274" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J274" s="6" t="s">
         <v>220</v>
       </c>
       <c r="L274" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D275" s="3"/>
       <c r="I275" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J275" s="6" t="s">
         <v>185</v>
       </c>
       <c r="L275" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D276" s="3"/>
       <c r="I276" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J276" s="6" t="s">
         <v>179</v>
       </c>
       <c r="L276" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D277" s="3"/>
       <c r="I277" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J277" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L277" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D278" s="3"/>
       <c r="I278" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J278" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="L278" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D279" s="3"/>
       <c r="I279" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="J279" s="6" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="L279" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C281" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D282" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E282" t="s">
         <v>20</v>
@@ -6472,12 +6472,12 @@
         <v>151</v>
       </c>
       <c r="L282" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D283" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E283" t="s">
         <v>20</v>
@@ -6486,12 +6486,12 @@
         <v>151</v>
       </c>
       <c r="L283" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D284" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E284" t="s">
         <v>20</v>
@@ -6500,25 +6500,25 @@
         <v>151</v>
       </c>
       <c r="L284" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A286" s="33" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B286" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C287" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D288" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E288" t="s">
         <v>4</v>
@@ -6527,12 +6527,12 @@
         <v>151</v>
       </c>
       <c r="L288" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="289" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D289" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E289" t="s">
         <v>20</v>
@@ -6541,12 +6541,12 @@
         <v>151</v>
       </c>
       <c r="L289" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="290" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D290" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E290" t="s">
         <v>4</v>
@@ -6555,12 +6555,12 @@
         <v>151</v>
       </c>
       <c r="L290" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="291" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D291" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E291" t="s">
         <v>20</v>
@@ -6569,12 +6569,12 @@
         <v>151</v>
       </c>
       <c r="L291" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="292" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D292" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E292" t="s">
         <v>20</v>
@@ -6583,12 +6583,12 @@
         <v>151</v>
       </c>
       <c r="L292" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="293" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D293" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E293" t="s">
         <v>20</v>
@@ -6597,154 +6597,154 @@
         <v>151</v>
       </c>
       <c r="L293" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="295" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C295" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="296" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D296" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E296" t="s">
         <v>4</v>
       </c>
       <c r="J296" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="297" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D297" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E297" t="s">
         <v>20</v>
       </c>
       <c r="J297" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="298" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D298" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E298" t="s">
         <v>4</v>
       </c>
       <c r="J298" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="299" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D299" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E299" t="s">
         <v>4</v>
       </c>
       <c r="J299" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="300" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D300" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E300" t="s">
         <v>4</v>
       </c>
       <c r="J300" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L300" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="301" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D301" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E301" t="s">
         <v>4</v>
       </c>
       <c r="J301" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L301" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="302" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D302" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E302" t="s">
         <v>4</v>
       </c>
       <c r="J302" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L302" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="303" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D303" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E303" t="s">
         <v>4</v>
       </c>
       <c r="J303" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L303" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="304" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D304" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E304" t="s">
         <v>4</v>
       </c>
       <c r="J304" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L304" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D305" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E305" t="s">
         <v>20</v>
       </c>
       <c r="J305" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L305" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E306" t="s">
         <v>20</v>
       </c>
       <c r="J306" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L306" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.3">
@@ -6752,215 +6752,215 @@
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A308" s="33" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B308" s="28" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="309" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C309" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D310" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E310" t="s">
         <v>4</v>
       </c>
       <c r="J310" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D311" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E311" t="s">
         <v>20</v>
       </c>
       <c r="J311" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D312" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E312" t="s">
         <v>20</v>
       </c>
       <c r="J312" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="313" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D313" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E313" t="s">
         <v>4</v>
       </c>
       <c r="J313" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D314" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E314" t="s">
         <v>4</v>
       </c>
       <c r="J314" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C316" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="317" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D317" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E317" t="s">
         <v>4</v>
       </c>
       <c r="J317" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L317" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D318" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E318" t="s">
         <v>20</v>
       </c>
       <c r="J318" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L318" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D319" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E319" t="s">
         <v>4</v>
       </c>
       <c r="J319" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L319" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D320" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E320" t="s">
         <v>4</v>
       </c>
       <c r="J320" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L320" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="321" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D321" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E321" t="s">
         <v>20</v>
       </c>
       <c r="J321" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L321" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="322" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D322" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E322" t="s">
         <v>20</v>
       </c>
       <c r="J322" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L322" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="323" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D323" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E323" t="s">
         <v>20</v>
       </c>
       <c r="J323" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L323" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="324" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D324" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E324" t="s">
         <v>20</v>
       </c>
       <c r="J324" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L324" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="325" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D325" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E325" t="s">
         <v>20</v>
       </c>
       <c r="J325" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L325" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="326" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D326" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E326" t="s">
         <v>20</v>
       </c>
       <c r="J326" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L326" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="327" spans="3:12" x14ac:dyDescent="0.3">
@@ -6971,85 +6971,85 @@
         <v>20</v>
       </c>
       <c r="J327" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L327" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="328" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D328" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E328" t="s">
         <v>4</v>
       </c>
       <c r="J328" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L328" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="329" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D329" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E329" t="s">
         <v>20</v>
       </c>
       <c r="J329" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L329" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="330" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D330" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E330" t="s">
         <v>20</v>
       </c>
       <c r="J330" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L330" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="331" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D331" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E331" t="s">
         <v>20</v>
       </c>
       <c r="J331" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L331" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="332" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D332" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E332" t="s">
         <v>20</v>
       </c>
       <c r="J332" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L332" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="333" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D333" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E333" t="s">
         <v>20</v>
@@ -7057,25 +7057,25 @@
     </row>
     <row r="335" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C335" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="336" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D336" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J336" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="338" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C338" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="339" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D339" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J339" t="s">
         <v>22</v>
@@ -7091,7 +7091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -7105,17 +7105,17 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
@@ -7126,51 +7126,51 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>491</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>6</v>
@@ -7185,10 +7185,10 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -7196,106 +7196,106 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C20" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D20" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E20" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="C21" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D21" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E21" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F21" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C22" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D22" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E22" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C23" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D23" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E23" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="F23" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C24" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="D24" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E24" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C25" t="s">
+        <v>497</v>
+      </c>
+      <c r="D25" t="s">
         <v>505</v>
       </c>
-      <c r="C25" t="s">
-        <v>502</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>510</v>
-      </c>
-      <c r="E25" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="C26" t="s">
         <v>511</v>
       </c>
-      <c r="C26" t="s">
-        <v>516</v>
-      </c>
       <c r="D26" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="E26" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>